<commit_message>
Finished NDepend analysis and included full report.
</commit_message>
<xml_diff>
--- a/data/fa_issues.xlsx
+++ b/data/fa_issues.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fa_issues" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="226">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -1429,13 +1429,14 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Category" numFmtId="0">
-      <sharedItems containsBlank="1" count="9">
+      <sharedItems containsBlank="1" count="10">
         <s v="Collections"/>
         <s v="Core"/>
         <s v="Equivalency"/>
         <s v="Events"/>
         <s v="Formatting"/>
         <s v="Primitives"/>
+        <s v="Specialized"/>
         <s v="Support"/>
         <s v="Updates"/>
         <m/>
@@ -1454,7 +1455,7 @@
     <x v="1"/>
     <x v="87"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="88"/>
@@ -1463,7 +1464,7 @@
     <x v="1"/>
     <x v="85"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="87"/>
@@ -1481,7 +1482,7 @@
     <x v="7"/>
     <x v="88"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="85"/>
@@ -1490,7 +1491,7 @@
     <x v="7"/>
     <x v="83"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="84"/>
@@ -1508,7 +1509,7 @@
     <x v="1"/>
     <x v="81"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="82"/>
@@ -1517,7 +1518,7 @@
     <x v="25"/>
     <x v="78"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="81"/>
@@ -1526,7 +1527,7 @@
     <x v="18"/>
     <x v="77"/>
     <x v="1"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="80"/>
@@ -1535,7 +1536,7 @@
     <x v="25"/>
     <x v="79"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="79"/>
@@ -1553,7 +1554,7 @@
     <x v="4"/>
     <x v="73"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="77"/>
@@ -1562,7 +1563,7 @@
     <x v="0"/>
     <x v="72"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="76"/>
@@ -1580,7 +1581,7 @@
     <x v="1"/>
     <x v="86"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="74"/>
@@ -1589,7 +1590,7 @@
     <x v="0"/>
     <x v="71"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="73"/>
@@ -1598,7 +1599,7 @@
     <x v="1"/>
     <x v="57"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="72"/>
@@ -1634,7 +1635,7 @@
     <x v="1"/>
     <x v="54"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="68"/>
@@ -1643,7 +1644,7 @@
     <x v="1"/>
     <x v="47"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="67"/>
@@ -1652,7 +1653,7 @@
     <x v="10"/>
     <x v="60"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="66"/>
@@ -1661,7 +1662,7 @@
     <x v="20"/>
     <x v="46"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="65"/>
@@ -1688,7 +1689,7 @@
     <x v="3"/>
     <x v="68"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="62"/>
@@ -1697,7 +1698,7 @@
     <x v="2"/>
     <x v="75"/>
     <x v="0"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="61"/>
@@ -1706,7 +1707,7 @@
     <x v="11"/>
     <x v="40"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="60"/>
@@ -1724,7 +1725,7 @@
     <x v="1"/>
     <x v="34"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="58"/>
@@ -1742,7 +1743,7 @@
     <x v="12"/>
     <x v="41"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="56"/>
@@ -1751,7 +1752,7 @@
     <x v="4"/>
     <x v="58"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="55"/>
@@ -1760,7 +1761,7 @@
     <x v="24"/>
     <x v="31"/>
     <x v="1"/>
-    <x v="7"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="54"/>
@@ -1778,7 +1779,7 @@
     <x v="12"/>
     <x v="32"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="52"/>
@@ -1787,7 +1788,7 @@
     <x v="11"/>
     <x v="49"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="51"/>
@@ -1796,7 +1797,7 @@
     <x v="11"/>
     <x v="30"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="50"/>
@@ -1805,7 +1806,7 @@
     <x v="25"/>
     <x v="21"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="49"/>
@@ -1814,7 +1815,7 @@
     <x v="25"/>
     <x v="20"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="48"/>
@@ -1823,7 +1824,7 @@
     <x v="12"/>
     <x v="27"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="47"/>
@@ -1832,7 +1833,7 @@
     <x v="25"/>
     <x v="18"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="46"/>
@@ -1841,7 +1842,7 @@
     <x v="25"/>
     <x v="53"/>
     <x v="0"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="45"/>
@@ -1859,7 +1860,7 @@
     <x v="11"/>
     <x v="17"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="43"/>
@@ -1868,7 +1869,7 @@
     <x v="11"/>
     <x v="16"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="42"/>
@@ -1895,7 +1896,7 @@
     <x v="11"/>
     <x v="35"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="39"/>
@@ -1904,7 +1905,7 @@
     <x v="25"/>
     <x v="39"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="38"/>
@@ -1922,7 +1923,7 @@
     <x v="25"/>
     <x v="11"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="36"/>
@@ -1931,7 +1932,7 @@
     <x v="25"/>
     <x v="29"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="35"/>
@@ -1940,7 +1941,7 @@
     <x v="25"/>
     <x v="9"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="34"/>
@@ -1958,7 +1959,7 @@
     <x v="9"/>
     <x v="44"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="32"/>
@@ -1967,7 +1968,7 @@
     <x v="25"/>
     <x v="8"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="31"/>
@@ -1976,7 +1977,7 @@
     <x v="11"/>
     <x v="19"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="30"/>
@@ -1994,7 +1995,7 @@
     <x v="25"/>
     <x v="6"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="28"/>
@@ -2003,7 +2004,7 @@
     <x v="1"/>
     <x v="67"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="27"/>
@@ -2039,7 +2040,7 @@
     <x v="17"/>
     <x v="59"/>
     <x v="1"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="23"/>
@@ -2048,7 +2049,7 @@
     <x v="11"/>
     <x v="51"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="22"/>
@@ -2057,7 +2058,7 @@
     <x v="15"/>
     <x v="70"/>
     <x v="1"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="21"/>
@@ -2066,7 +2067,7 @@
     <x v="25"/>
     <x v="36"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="20"/>
@@ -2075,7 +2076,7 @@
     <x v="25"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="19"/>
@@ -2084,7 +2085,7 @@
     <x v="15"/>
     <x v="15"/>
     <x v="1"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="18"/>
@@ -2093,7 +2094,7 @@
     <x v="6"/>
     <x v="4"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="17"/>
@@ -2102,7 +2103,7 @@
     <x v="15"/>
     <x v="69"/>
     <x v="1"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="16"/>
@@ -2120,7 +2121,7 @@
     <x v="11"/>
     <x v="64"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="14"/>
@@ -2138,7 +2139,7 @@
     <x v="11"/>
     <x v="7"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="12"/>
@@ -2147,7 +2148,7 @@
     <x v="22"/>
     <x v="28"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="11"/>
@@ -2156,7 +2157,7 @@
     <x v="15"/>
     <x v="14"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="10"/>
@@ -2165,7 +2166,7 @@
     <x v="9"/>
     <x v="26"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="9"/>
@@ -2174,7 +2175,7 @@
     <x v="11"/>
     <x v="5"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="8"/>
@@ -2183,7 +2184,7 @@
     <x v="11"/>
     <x v="45"/>
     <x v="0"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="7"/>
@@ -2192,7 +2193,7 @@
     <x v="11"/>
     <x v="42"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="6"/>
@@ -2210,7 +2211,7 @@
     <x v="11"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="4"/>
@@ -2228,7 +2229,7 @@
     <x v="15"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="2"/>
@@ -2237,7 +2238,7 @@
     <x v="11"/>
     <x v="25"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="1"/>
@@ -2246,7 +2247,7 @@
     <x v="15"/>
     <x v="62"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
@@ -2255,14 +2256,14 @@
     <x v="11"/>
     <x v="24"/>
     <x v="1"/>
-    <x v="8"/>
+    <x v="9"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="0" outlineData="0" compact="0" compactData="0">
-  <location ref="A1:D12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A1:D13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" compact="0" showAll="0" outline="0"/>
     <pivotField compact="0" showAll="0"/>
@@ -2276,16 +2277,17 @@
       </items>
     </pivotField>
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0" outline="0">
-      <items count="9">
+      <items count="10">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
-        <item x="6"/>
         <item x="7"/>
         <item x="8"/>
+        <item x="9"/>
+        <item x="6"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -2309,8 +2311,8 @@
   </sheetPr>
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E94" activeCellId="0" sqref="E93:E94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E94" activeCellId="0" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2431,7 +2433,7 @@
         <f aca="false">VLOOKUP(A5,fa_milestone_issues!A:C,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2455,7 +2457,7 @@
         <f aca="false">VLOOKUP(A6,fa_milestone_issues!A:C,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2608,7 +2610,7 @@
         <f aca="false">VLOOKUP(A13,fa_milestone_issues!A:C,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2854,7 +2856,7 @@
         <f aca="false">VLOOKUP(A24,fa_milestone_issues!A:C,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="G24" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3100,7 +3102,7 @@
         <f aca="false">VLOOKUP(A35,fa_milestone_issues!A:C,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="G35" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3910,7 +3912,7 @@
         <f aca="false">VLOOKUP(A73,fa_milestone_issues!A:C,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G73" s="0" t="s">
+      <c r="G73" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4069,7 +4071,7 @@
         <f aca="false">VLOOKUP(A80,fa_milestone_issues!A:C,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G80" s="0" t="s">
+      <c r="G80" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4246,7 +4248,7 @@
         <f aca="false">VLOOKUP(A88,fa_milestone_issues!A:C,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G88" s="0" t="s">
+      <c r="G88" s="3" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4291,7 +4293,7 @@
         <f aca="false">VLOOKUP(A90,fa_milestone_issues!A:C,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G90" s="0" t="s">
+      <c r="G90" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4346,10 +4348,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="E93:E94 B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4400,10 +4402,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="19" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4414,10 +4416,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="18" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D5" s="19" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4426,10 +4428,10 @@
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6" s="19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4438,10 +4440,10 @@
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4488,27 +4490,39 @@
       <c r="A11" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="B11" s="20" t="n">
+      <c r="B11" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="21" t="n">
-        <v>56</v>
-      </c>
-      <c r="D11" s="22" t="n">
-        <v>58</v>
+      <c r="C11" s="18" t="n">
+        <v>47</v>
+      </c>
+      <c r="D11" s="19" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="B12" s="24" t="n">
+      <c r="B13" s="24" t="n">
         <v>13</v>
       </c>
-      <c r="C12" s="25" t="n">
+      <c r="C13" s="25" t="n">
         <v>77</v>
       </c>
-      <c r="D12" s="26" t="n">
+      <c r="D13" s="26" t="n">
         <v>90</v>
       </c>
     </row>
@@ -4531,7 +4545,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="E93:E94 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>